<commit_message>
Toevoeging van details in "opmerkingen" sectie (meer detail teogevoegd)
meer detail toegevoegd aan "Opmerkingen" sectie van de productiviteit.
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -85,10 +85,10 @@
     <t>Naam : Jorrit Verheul</t>
   </si>
   <si>
-    <t>Opzetten van de werk omgeving en ervoor gezorgd dat alles werkt in combinatie met Github</t>
+    <t>Plan van aanpak maken en laten nakijken of deze goed is.</t>
   </si>
   <si>
-    <t>Plan van aanpak maken en laten nakijken of deze goed is.</t>
+    <t>Opzetten van de werk omgeving en ervoor gezorgd dat alles werkt in combinatie met Github en gesprek met opdrachtgeven (Paul Jurriens) gehad over het concept.</t>
   </si>
 </sst>
 </file>
@@ -646,6 +646,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -657,12 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,7 +996,7 @@
   <dimension ref="B2:H53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1097,17 +1097,17 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="60"/>
       <c r="G12" s="26"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="2:8" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="B13" s="55" t="s">
         <v>6</v>
       </c>
@@ -1118,8 +1118,8 @@
         <v>6</v>
       </c>
       <c r="E13" s="42"/>
-      <c r="F13" s="74" t="s">
-        <v>22</v>
+      <c r="F13" s="70" t="s">
+        <v>23</v>
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
@@ -1133,8 +1133,8 @@
       </c>
       <c r="D14" s="46"/>
       <c r="E14" s="46"/>
-      <c r="F14" s="75" t="s">
-        <v>23</v>
+      <c r="F14" s="71" t="s">
+        <v>22</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="17"/>
@@ -1518,10 +1518,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="71"/>
+      <c r="C46" s="73"/>
       <c r="D46" s="33"/>
       <c r="E46" s="69" t="s">
         <v>13</v>
@@ -1719,10 +1719,10 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="2:10" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="40"/>
@@ -2378,15 +2378,15 @@
       <c r="J45" s="18"/>
     </row>
     <row r="46" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="71"/>
+      <c r="C46" s="73"/>
       <c r="D46" s="67"/>
-      <c r="E46" s="70" t="s">
+      <c r="E46" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="71"/>
+      <c r="F46" s="73"/>
       <c r="G46" s="3"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
@@ -2595,10 +2595,10 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="2:10" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="40"/>
@@ -3254,15 +3254,15 @@
       <c r="J45" s="18"/>
     </row>
     <row r="46" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="71"/>
+      <c r="C46" s="73"/>
       <c r="D46" s="67"/>
-      <c r="E46" s="70" t="s">
+      <c r="E46" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="71"/>
+      <c r="F46" s="73"/>
       <c r="G46" s="3"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
@@ -3471,10 +3471,10 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="2:10" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="40"/>
@@ -4130,15 +4130,15 @@
       <c r="J45" s="18"/>
     </row>
     <row r="46" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="71"/>
+      <c r="C46" s="73"/>
       <c r="D46" s="67"/>
-      <c r="E46" s="70" t="s">
+      <c r="E46" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="71"/>
+      <c r="F46" s="73"/>
       <c r="G46" s="3"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>

</xml_diff>

<commit_message>
Urenverantwoording bijgewerkt Informatiebehoefte (WIP) bestand toegevoegd
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menno\Documents\Wijkertoren-docs\Uren Verantwoording\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Uren Jeffrey Meyer" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Uren Roel Meijns" sheetId="3" r:id="rId3"/>
     <sheet name="Uren Jorrit Verheul" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -86,6 +91,12 @@
   </si>
   <si>
     <t xml:space="preserve">Plan van aanpak maken en laten nakijken of deze goed is. Github problemen (merge conflict gefixed) </t>
+  </si>
+  <si>
+    <t>Informatiebehoefte uitwerken</t>
+  </si>
+  <si>
+    <t>Opzetten project, interview regelen, interview houden</t>
   </si>
 </sst>
 </file>
@@ -359,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -530,6 +541,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -542,16 +559,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -595,9 +615,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -635,9 +655,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -672,7 +692,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -707,7 +727,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -883,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -985,10 +1005,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -1002,7 +1022,7 @@
       <c r="C13" s="56">
         <v>42772</v>
       </c>
-      <c r="D13" s="66">
+      <c r="D13" s="62">
         <v>6</v>
       </c>
       <c r="E13" s="39"/>
@@ -1019,7 +1039,7 @@
       <c r="C14" s="56">
         <v>42773</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="63">
         <v>4</v>
       </c>
       <c r="E14" s="41"/>
@@ -1036,7 +1056,7 @@
       <c r="C15" s="56">
         <v>42774</v>
       </c>
-      <c r="D15" s="67"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="41"/>
       <c r="F15" s="51"/>
       <c r="G15" s="27"/>
@@ -1049,7 +1069,7 @@
       <c r="C16" s="56">
         <v>42775</v>
       </c>
-      <c r="D16" s="67"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="41"/>
       <c r="F16" s="51"/>
       <c r="G16" s="27"/>
@@ -1062,7 +1082,7 @@
       <c r="C17" s="56">
         <v>42776</v>
       </c>
-      <c r="D17" s="67"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="41"/>
       <c r="F17" s="51"/>
       <c r="G17" s="27"/>
@@ -1408,10 +1428,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="63"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="33"/>
       <c r="E46" s="57" t="s">
         <v>11</v>
@@ -1481,15 +1501,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="23"/>
-    <col min="3" max="3" width="8.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.85546875" style="13" customWidth="1"/>
     <col min="6" max="6" width="33" style="54" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="54" customWidth="1"/>
@@ -1583,24 +1603,30 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
       <c r="G12" s="26"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="2:8" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="39"/>
+      <c r="C13" s="56">
+        <v>42772</v>
+      </c>
+      <c r="D13" s="39">
+        <v>6</v>
+      </c>
       <c r="E13" s="39"/>
-      <c r="F13" s="50"/>
+      <c r="F13" s="68" t="s">
+        <v>24</v>
+      </c>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
@@ -1608,10 +1634,16 @@
       <c r="B14" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="41"/>
+      <c r="C14" s="56">
+        <v>42773</v>
+      </c>
+      <c r="D14" s="41">
+        <v>4</v>
+      </c>
       <c r="E14" s="41"/>
-      <c r="F14" s="51"/>
+      <c r="F14" s="69" t="s">
+        <v>23</v>
+      </c>
       <c r="G14" s="27"/>
       <c r="H14" s="17"/>
     </row>
@@ -1619,10 +1651,12 @@
       <c r="B15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="56"/>
+      <c r="C15" s="56">
+        <v>42774</v>
+      </c>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
-      <c r="F15" s="51"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="27"/>
       <c r="H15" s="18"/>
     </row>
@@ -1630,10 +1664,12 @@
       <c r="B16" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="56"/>
+      <c r="C16" s="56">
+        <v>42775</v>
+      </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
-      <c r="F16" s="51"/>
+      <c r="F16" s="69"/>
       <c r="G16" s="27"/>
       <c r="H16" s="18"/>
     </row>
@@ -1641,10 +1677,12 @@
       <c r="B17" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="56"/>
+      <c r="C17" s="56">
+        <v>42776</v>
+      </c>
       <c r="D17" s="41"/>
       <c r="E17" s="41"/>
-      <c r="F17" s="51"/>
+      <c r="F17" s="69"/>
       <c r="G17" s="27"/>
       <c r="H17" s="18"/>
     </row>
@@ -1655,13 +1693,13 @@
       <c r="C18" s="42"/>
       <c r="D18" s="43">
         <f>SUM(D13:D17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E18" s="43">
         <f>SUM(E13:E17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="52"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="28"/>
       <c r="H18" s="19"/>
     </row>
@@ -1669,10 +1707,12 @@
       <c r="B19" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="56"/>
+      <c r="C19" s="56">
+        <v>42779</v>
+      </c>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
-      <c r="F19" s="50"/>
+      <c r="F19" s="68"/>
       <c r="G19" s="27"/>
       <c r="H19" s="18"/>
     </row>
@@ -1680,10 +1720,12 @@
       <c r="B20" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="56"/>
+      <c r="C20" s="56">
+        <v>42780</v>
+      </c>
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
-      <c r="F20" s="51"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="27"/>
       <c r="H20" s="18"/>
     </row>
@@ -1691,10 +1733,12 @@
       <c r="B21" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="56"/>
+      <c r="C21" s="56">
+        <v>42781</v>
+      </c>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
-      <c r="F21" s="51"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="27"/>
       <c r="H21" s="18"/>
     </row>
@@ -1702,10 +1746,12 @@
       <c r="B22" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="56"/>
+      <c r="C22" s="56">
+        <v>42782</v>
+      </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
-      <c r="F22" s="51"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="27"/>
       <c r="H22" s="18"/>
     </row>
@@ -1713,10 +1759,12 @@
       <c r="B23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="56">
+        <v>42783</v>
+      </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
-      <c r="F23" s="51"/>
+      <c r="F23" s="69"/>
       <c r="G23" s="27"/>
       <c r="H23" s="18"/>
     </row>
@@ -1733,7 +1781,7 @@
         <f>SUM(E19:E23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="52"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="28"/>
       <c r="H24" s="19"/>
     </row>
@@ -1741,10 +1789,12 @@
       <c r="B25" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="56"/>
+      <c r="C25" s="56">
+        <v>42786</v>
+      </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
-      <c r="F25" s="50"/>
+      <c r="F25" s="68"/>
       <c r="G25" s="27"/>
       <c r="H25" s="18"/>
     </row>
@@ -1752,10 +1802,12 @@
       <c r="B26" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="56"/>
+      <c r="C26" s="56">
+        <v>42787</v>
+      </c>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="27"/>
       <c r="H26" s="18"/>
     </row>
@@ -1763,10 +1815,12 @@
       <c r="B27" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="56"/>
+      <c r="C27" s="56">
+        <v>42788</v>
+      </c>
       <c r="D27" s="41"/>
       <c r="E27" s="41"/>
-      <c r="F27" s="51"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="27"/>
       <c r="H27" s="18"/>
     </row>
@@ -1774,10 +1828,12 @@
       <c r="B28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="56"/>
+      <c r="C28" s="56">
+        <v>42789</v>
+      </c>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
-      <c r="F28" s="51"/>
+      <c r="F28" s="69"/>
       <c r="G28" s="27"/>
       <c r="H28" s="18"/>
     </row>
@@ -1785,10 +1841,12 @@
       <c r="B29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="56"/>
+      <c r="C29" s="56">
+        <v>42790</v>
+      </c>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
-      <c r="F29" s="51"/>
+      <c r="F29" s="69"/>
       <c r="G29" s="27"/>
       <c r="H29" s="18"/>
     </row>
@@ -1796,7 +1854,7 @@
       <c r="B30" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="56"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="43">
         <f>SUM(D25:D29)</f>
         <v>0</v>
@@ -1805,7 +1863,7 @@
         <f>SUM(E25:E29)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="52"/>
+      <c r="F30" s="70"/>
       <c r="G30" s="28"/>
       <c r="H30" s="19"/>
     </row>
@@ -1813,10 +1871,12 @@
       <c r="B31" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="C31" s="56">
+        <v>42793</v>
+      </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
-      <c r="F31" s="50"/>
+      <c r="F31" s="68"/>
       <c r="G31" s="27"/>
       <c r="H31" s="18"/>
     </row>
@@ -1824,10 +1884,12 @@
       <c r="B32" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="56"/>
+      <c r="C32" s="56">
+        <v>42794</v>
+      </c>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
-      <c r="F32" s="51"/>
+      <c r="F32" s="69"/>
       <c r="G32" s="27"/>
       <c r="H32" s="18"/>
     </row>
@@ -1835,10 +1897,12 @@
       <c r="B33" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="56"/>
+      <c r="C33" s="56">
+        <v>42795</v>
+      </c>
       <c r="D33" s="41"/>
       <c r="E33" s="41"/>
-      <c r="F33" s="51"/>
+      <c r="F33" s="69"/>
       <c r="G33" s="27"/>
       <c r="H33" s="18"/>
     </row>
@@ -1846,10 +1910,12 @@
       <c r="B34" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="56"/>
+      <c r="C34" s="56">
+        <v>42796</v>
+      </c>
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
-      <c r="F34" s="51"/>
+      <c r="F34" s="69"/>
       <c r="G34" s="27"/>
       <c r="H34" s="18"/>
     </row>
@@ -1857,10 +1923,12 @@
       <c r="B35" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="40"/>
+      <c r="C35" s="56">
+        <v>42797</v>
+      </c>
       <c r="D35" s="41"/>
       <c r="E35" s="41"/>
-      <c r="F35" s="51"/>
+      <c r="F35" s="69"/>
       <c r="G35" s="27"/>
       <c r="H35" s="18"/>
     </row>
@@ -1877,7 +1945,7 @@
         <f>SUM(E31:E35)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="52"/>
+      <c r="F36" s="70"/>
       <c r="G36" s="28"/>
       <c r="H36" s="19"/>
     </row>
@@ -1885,10 +1953,12 @@
       <c r="B37" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="56"/>
+      <c r="C37" s="56">
+        <v>42800</v>
+      </c>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
-      <c r="F37" s="50"/>
+      <c r="F37" s="68"/>
       <c r="G37" s="27"/>
       <c r="H37" s="18"/>
     </row>
@@ -1896,10 +1966,12 @@
       <c r="B38" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="56"/>
+      <c r="C38" s="56">
+        <v>42801</v>
+      </c>
       <c r="D38" s="41"/>
       <c r="E38" s="41"/>
-      <c r="F38" s="51"/>
+      <c r="F38" s="69"/>
       <c r="G38" s="27"/>
       <c r="H38" s="18"/>
     </row>
@@ -1907,10 +1979,12 @@
       <c r="B39" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="56"/>
+      <c r="C39" s="56">
+        <v>42802</v>
+      </c>
       <c r="D39" s="41"/>
       <c r="E39" s="41"/>
-      <c r="F39" s="51"/>
+      <c r="F39" s="69"/>
       <c r="G39" s="27"/>
       <c r="H39" s="18"/>
     </row>
@@ -1918,10 +1992,12 @@
       <c r="B40" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="56"/>
+      <c r="C40" s="56">
+        <v>42803</v>
+      </c>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
-      <c r="F40" s="51"/>
+      <c r="F40" s="69"/>
       <c r="G40" s="27"/>
       <c r="H40" s="18"/>
     </row>
@@ -1929,10 +2005,12 @@
       <c r="B41" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="56"/>
+      <c r="C41" s="56">
+        <v>42804</v>
+      </c>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
-      <c r="F41" s="51"/>
+      <c r="F41" s="69"/>
       <c r="G41" s="27"/>
       <c r="H41" s="18"/>
     </row>
@@ -1949,7 +2027,7 @@
         <f>SUM(E37:E41)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="52"/>
+      <c r="F42" s="70"/>
       <c r="G42" s="28"/>
       <c r="H42" s="19"/>
     </row>
@@ -1960,7 +2038,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E43" s="36">
         <f>SUM(E18+E24+E30+E36+E42)</f>
@@ -1988,10 +2066,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="63"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="55"/>
       <c r="E46" s="60" t="s">
         <v>11</v>
@@ -2053,6 +2131,7 @@
     <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2162,10 +2241,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -2567,10 +2646,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="63"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="55"/>
       <c r="E46" s="60" t="s">
         <v>11</v>
@@ -2741,10 +2820,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -3200,10 +3279,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="63"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="55"/>
       <c r="E46" s="60" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Informatiebehoefde moet nagekeken worden. Uren verantwoording aangepast
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Opzetten project, interview regelen, interview houden</t>
+  </si>
+  <si>
+    <t>Informatiebehoefte "afgemaakt", 2e interview gedaan.</t>
   </si>
 </sst>
 </file>
@@ -547,6 +550,15 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -558,15 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,10 +1008,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -1428,10 +1431,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="65"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="33"/>
       <c r="E46" s="57" t="s">
         <v>11</v>
@@ -1502,7 +1505,7 @@
   <dimension ref="B2:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1603,10 +1606,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -1624,13 +1627,13 @@
         <v>6</v>
       </c>
       <c r="E13" s="39"/>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="64" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" spans="2:8" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="45" t="s">
         <v>6</v>
       </c>
@@ -1641,22 +1644,26 @@
         <v>4</v>
       </c>
       <c r="E14" s="41"/>
-      <c r="F14" s="69" t="s">
+      <c r="F14" s="65" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="24" x14ac:dyDescent="0.2">
       <c r="B15" s="45" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="56">
         <v>42774</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="41">
+        <v>4</v>
+      </c>
       <c r="E15" s="41"/>
-      <c r="F15" s="69"/>
+      <c r="F15" s="65" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" s="27"/>
       <c r="H15" s="18"/>
     </row>
@@ -1669,7 +1676,7 @@
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
-      <c r="F16" s="69"/>
+      <c r="F16" s="65"/>
       <c r="G16" s="27"/>
       <c r="H16" s="18"/>
     </row>
@@ -1682,7 +1689,7 @@
       </c>
       <c r="D17" s="41"/>
       <c r="E17" s="41"/>
-      <c r="F17" s="69"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="27"/>
       <c r="H17" s="18"/>
     </row>
@@ -1693,13 +1700,13 @@
       <c r="C18" s="42"/>
       <c r="D18" s="43">
         <f>SUM(D13:D17)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E18" s="43">
         <f>SUM(E13:E17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="70"/>
+      <c r="F18" s="66"/>
       <c r="G18" s="28"/>
       <c r="H18" s="19"/>
     </row>
@@ -1712,7 +1719,7 @@
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
-      <c r="F19" s="68"/>
+      <c r="F19" s="64"/>
       <c r="G19" s="27"/>
       <c r="H19" s="18"/>
     </row>
@@ -1725,7 +1732,7 @@
       </c>
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
-      <c r="F20" s="69"/>
+      <c r="F20" s="65"/>
       <c r="G20" s="27"/>
       <c r="H20" s="18"/>
     </row>
@@ -1738,7 +1745,7 @@
       </c>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
-      <c r="F21" s="69"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="27"/>
       <c r="H21" s="18"/>
     </row>
@@ -1751,7 +1758,7 @@
       </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
-      <c r="F22" s="69"/>
+      <c r="F22" s="65"/>
       <c r="G22" s="27"/>
       <c r="H22" s="18"/>
     </row>
@@ -1764,7 +1771,7 @@
       </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
-      <c r="F23" s="69"/>
+      <c r="F23" s="65"/>
       <c r="G23" s="27"/>
       <c r="H23" s="18"/>
     </row>
@@ -1781,7 +1788,7 @@
         <f>SUM(E19:E23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="70"/>
+      <c r="F24" s="66"/>
       <c r="G24" s="28"/>
       <c r="H24" s="19"/>
     </row>
@@ -1794,7 +1801,7 @@
       </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
-      <c r="F25" s="68"/>
+      <c r="F25" s="64"/>
       <c r="G25" s="27"/>
       <c r="H25" s="18"/>
     </row>
@@ -1807,7 +1814,7 @@
       </c>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
-      <c r="F26" s="69"/>
+      <c r="F26" s="65"/>
       <c r="G26" s="27"/>
       <c r="H26" s="18"/>
     </row>
@@ -1820,7 +1827,7 @@
       </c>
       <c r="D27" s="41"/>
       <c r="E27" s="41"/>
-      <c r="F27" s="69"/>
+      <c r="F27" s="65"/>
       <c r="G27" s="27"/>
       <c r="H27" s="18"/>
     </row>
@@ -1833,7 +1840,7 @@
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
-      <c r="F28" s="69"/>
+      <c r="F28" s="65"/>
       <c r="G28" s="27"/>
       <c r="H28" s="18"/>
     </row>
@@ -1846,7 +1853,7 @@
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
-      <c r="F29" s="69"/>
+      <c r="F29" s="65"/>
       <c r="G29" s="27"/>
       <c r="H29" s="18"/>
     </row>
@@ -1863,7 +1870,7 @@
         <f>SUM(E25:E29)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="70"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="28"/>
       <c r="H30" s="19"/>
     </row>
@@ -1876,7 +1883,7 @@
       </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
-      <c r="F31" s="68"/>
+      <c r="F31" s="64"/>
       <c r="G31" s="27"/>
       <c r="H31" s="18"/>
     </row>
@@ -1889,7 +1896,7 @@
       </c>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
-      <c r="F32" s="69"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="27"/>
       <c r="H32" s="18"/>
     </row>
@@ -1902,7 +1909,7 @@
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="41"/>
-      <c r="F33" s="69"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="27"/>
       <c r="H33" s="18"/>
     </row>
@@ -1915,7 +1922,7 @@
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
-      <c r="F34" s="69"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="27"/>
       <c r="H34" s="18"/>
     </row>
@@ -1928,7 +1935,7 @@
       </c>
       <c r="D35" s="41"/>
       <c r="E35" s="41"/>
-      <c r="F35" s="69"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="27"/>
       <c r="H35" s="18"/>
     </row>
@@ -1945,7 +1952,7 @@
         <f>SUM(E31:E35)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="70"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="28"/>
       <c r="H36" s="19"/>
     </row>
@@ -1958,7 +1965,7 @@
       </c>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
-      <c r="F37" s="68"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="27"/>
       <c r="H37" s="18"/>
     </row>
@@ -1971,7 +1978,7 @@
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="41"/>
-      <c r="F38" s="69"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="27"/>
       <c r="H38" s="18"/>
     </row>
@@ -1984,7 +1991,7 @@
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="41"/>
-      <c r="F39" s="69"/>
+      <c r="F39" s="65"/>
       <c r="G39" s="27"/>
       <c r="H39" s="18"/>
     </row>
@@ -1997,7 +2004,7 @@
       </c>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
-      <c r="F40" s="69"/>
+      <c r="F40" s="65"/>
       <c r="G40" s="27"/>
       <c r="H40" s="18"/>
     </row>
@@ -2010,7 +2017,7 @@
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
-      <c r="F41" s="69"/>
+      <c r="F41" s="65"/>
       <c r="G41" s="27"/>
       <c r="H41" s="18"/>
     </row>
@@ -2027,7 +2034,7 @@
         <f>SUM(E37:E41)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="70"/>
+      <c r="F42" s="66"/>
       <c r="G42" s="28"/>
       <c r="H42" s="19"/>
     </row>
@@ -2038,7 +2045,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E43" s="36">
         <f>SUM(E18+E24+E30+E36+E42)</f>
@@ -2066,10 +2073,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="65"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="55"/>
       <c r="E46" s="60" t="s">
         <v>11</v>
@@ -2241,10 +2248,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -2646,10 +2653,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="65"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="55"/>
       <c r="E46" s="60" t="s">
         <v>11</v>
@@ -2820,10 +2827,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="49"/>
@@ -3279,10 +3286,10 @@
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="65"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="55"/>
       <c r="E46" s="60" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Uren verantwoording van Maandag 13-2-2017 ingevuld
Uren verantwoording van Maandag 13-2-2017 ingevuld.
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="33">
   <si>
     <t>Datum</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Plan van aanpak maken en laten nakijken of deze goed is. Github problemen (merge conflict gefixed).</t>
+  </si>
+  <si>
+    <t>Extern hulp verleent en met Menno v. Zijtveld normalisatie gemaakt morgen Dinsdag 14-2-2017 mee verder gaan.</t>
   </si>
 </sst>
 </file>
@@ -920,7 +923,7 @@
   <dimension ref="B2:H53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1129,14 +1132,20 @@
       <c r="G18" s="28"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="36" x14ac:dyDescent="0.2">
       <c r="B19" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="39"/>
+      <c r="C19" s="56">
+        <v>42779</v>
+      </c>
+      <c r="D19" s="39">
+        <v>7</v>
+      </c>
       <c r="E19" s="39"/>
-      <c r="F19" s="50"/>
+      <c r="F19" s="58" t="s">
+        <v>32</v>
+      </c>
       <c r="G19" s="27"/>
       <c r="H19" s="18"/>
     </row>
@@ -1144,7 +1153,9 @@
       <c r="B20" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="56"/>
+      <c r="C20" s="56">
+        <v>42780</v>
+      </c>
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
       <c r="F20" s="51"/>
@@ -1155,7 +1166,9 @@
       <c r="B21" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="56"/>
+      <c r="C21" s="56">
+        <v>42781</v>
+      </c>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
       <c r="F21" s="51"/>
@@ -1166,7 +1179,9 @@
       <c r="B22" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="56"/>
+      <c r="C22" s="56">
+        <v>42782</v>
+      </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
       <c r="F22" s="51"/>
@@ -1177,7 +1192,9 @@
       <c r="B23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="56">
+        <v>42783</v>
+      </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
       <c r="F23" s="51"/>
@@ -1191,7 +1208,7 @@
       <c r="C24" s="42"/>
       <c r="D24" s="43">
         <f>SUM(D19:D23)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E24" s="43">
         <f>SUM(E19:E23)</f>
@@ -1424,7 +1441,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E43" s="36">
         <f>SUM(E18+E24+E30+E36+E42)</f>

</xml_diff>

<commit_message>
Update Urenverantwoording inclusief Engels examen voorbereiding
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -129,7 +129,7 @@
     <t>Normaliseren database</t>
   </si>
   <si>
-    <t>Afmaken kerntaak 1, plannen voor kerntaak 2</t>
+    <t>Afmaken kerntaak 1, plannen voor kerntaak 2 (2uur Engels examen voorbereiden)</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +1785,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="2:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" ht="36" x14ac:dyDescent="0.2">
       <c r="B16" s="45" t="s">
         <v>8</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>42775</v>
       </c>
       <c r="D16" s="41">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
@@ -1826,7 +1826,7 @@
       <c r="C18" s="42"/>
       <c r="D18" s="43">
         <f>SUM(D13:D17)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="43">
         <f>SUM(E13:E17)</f>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="36">

</xml_diff>

<commit_message>
Paar dingetjes gefixt in Uren verantwoording
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menno\Documents\Wijkertoren-docs\Uren Verantwoording\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Uren Jeffrey Meyer" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="Uren Roel Meijns" sheetId="3" r:id="rId3"/>
     <sheet name="Uren Jorrit Verheul" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="34">
   <si>
     <t>Datum</t>
   </si>
@@ -52,9 +47,6 @@
   </si>
   <si>
     <t>Vrijdag</t>
-  </si>
-  <si>
-    <t>Saldo week</t>
   </si>
   <si>
     <t>Handtekening leidinggevende :</t>
@@ -126,10 +118,7 @@
     <t>Rooster Vrij</t>
   </si>
   <si>
-    <t>Normaliseren database</t>
-  </si>
-  <si>
-    <t>Afmaken kerntaak 1, plannen voor kerntaak 2 (2uur Engels examen voorbereiden)</t>
+    <t>Uur week</t>
   </si>
 </sst>
 </file>
@@ -606,8 +595,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -651,9 +640,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -691,9 +680,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -728,7 +717,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,7 +752,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -939,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -956,7 +945,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -976,7 +965,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="29"/>
@@ -1035,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>2</v>
@@ -1048,7 +1037,7 @@
     </row>
     <row r="12" spans="2:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="34"/>
@@ -1071,7 +1060,7 @@
       <c r="E13" s="62"/>
       <c r="F13" s="39"/>
       <c r="G13" s="58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
@@ -1089,7 +1078,7 @@
       <c r="E14" s="63"/>
       <c r="F14" s="41"/>
       <c r="G14" s="59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="17"/>
@@ -1107,7 +1096,7 @@
       <c r="E15" s="63"/>
       <c r="F15" s="41"/>
       <c r="G15" s="59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
@@ -1125,7 +1114,7 @@
       <c r="E16" s="63"/>
       <c r="F16" s="41"/>
       <c r="G16" s="65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
@@ -1148,7 +1137,7 @@
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43">
@@ -1180,7 +1169,7 @@
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
       <c r="G19" s="58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
@@ -1243,7 +1232,7 @@
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="43">
@@ -1321,7 +1310,7 @@
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="43">
@@ -1399,7 +1388,7 @@
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="43">
@@ -1477,7 +1466,7 @@
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43">
@@ -1532,13 +1521,13 @@
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="33"/>
       <c r="E46" s="67"/>
       <c r="F46" s="57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
@@ -1612,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H16:H17"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B42" sqref="B18:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1618,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1649,7 +1638,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="29"/>
@@ -1708,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>2</v>
@@ -1721,7 +1710,7 @@
     </row>
     <row r="12" spans="2:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="34"/>
@@ -1744,7 +1733,7 @@
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
       <c r="G13" s="64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
@@ -1762,7 +1751,7 @@
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
       <c r="G14" s="65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="17"/>
@@ -1780,26 +1769,22 @@
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
       <c r="G15" s="65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="2:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="45" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="56">
         <v>42775</v>
       </c>
-      <c r="D16" s="41">
-        <v>5</v>
-      </c>
+      <c r="D16" s="41"/>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
-      <c r="G16" s="65" t="s">
-        <v>35</v>
-      </c>
+      <c r="G16" s="65"/>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
     </row>
@@ -1821,12 +1806,12 @@
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43">
         <f>SUM(D13:D17)</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E18" s="43">
         <f>SUM(E13:E17)</f>
@@ -1847,14 +1832,10 @@
       <c r="C19" s="56">
         <v>42779</v>
       </c>
-      <c r="D19" s="39">
-        <v>6</v>
-      </c>
+      <c r="D19" s="39"/>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="64" t="s">
-        <v>34</v>
-      </c>
+      <c r="G19" s="64"/>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
     </row>
@@ -1868,9 +1849,7 @@
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="65" t="s">
-        <v>34</v>
-      </c>
+      <c r="G20" s="65"/>
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
@@ -1918,12 +1897,12 @@
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="43">
         <f>SUM(D19:D23)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E24" s="43"/>
       <c r="F24" s="43">
@@ -2006,7 +1985,7 @@
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C30" s="42"/>
       <c r="D30" s="43">
@@ -2094,7 +2073,7 @@
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="43">
@@ -2182,7 +2161,7 @@
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43">
@@ -2205,7 +2184,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="36">
@@ -2237,13 +2216,13 @@
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="55"/>
       <c r="E46" s="67"/>
       <c r="F46" s="60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
@@ -2318,7 +2297,7 @@
   <dimension ref="A2:I53"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B18" sqref="B18:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2334,7 +2313,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2354,7 +2333,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="29"/>
@@ -2413,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>2</v>
@@ -2426,7 +2405,7 @@
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="34"/>
@@ -2449,7 +2428,7 @@
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
       <c r="G13" s="58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
@@ -2484,7 +2463,7 @@
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
       <c r="G15" s="59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
@@ -2502,7 +2481,7 @@
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
       <c r="G16" s="59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
@@ -2520,14 +2499,14 @@
       <c r="E17" s="41"/>
       <c r="F17" s="41"/>
       <c r="G17" s="59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43">
@@ -2608,7 +2587,7 @@
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="43">
@@ -2686,7 +2665,7 @@
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="43">
@@ -2764,7 +2743,7 @@
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="43">
@@ -2842,7 +2821,7 @@
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43">
@@ -2897,13 +2876,13 @@
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="55"/>
       <c r="E46" s="67"/>
       <c r="F46" s="60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
@@ -2976,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2993,7 +2972,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3013,7 +2992,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="29"/>
@@ -3072,7 +3051,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>2</v>
@@ -3085,7 +3064,7 @@
     </row>
     <row r="12" spans="2:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="34"/>
@@ -3108,7 +3087,7 @@
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
       <c r="G13" s="50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
@@ -3171,7 +3150,7 @@
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43">
@@ -3262,7 +3241,7 @@
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="43">
@@ -3350,7 +3329,7 @@
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="43">
@@ -3438,7 +3417,7 @@
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="43">
@@ -3526,7 +3505,7 @@
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="46" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43">
@@ -3581,13 +3560,13 @@
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="55"/>
       <c r="E46" s="67"/>
       <c r="F46" s="60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>

</xml_diff>

<commit_message>
urenverantwoording t/m 14-2 Menno
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menno\Documents\Wijkertoren-docs\Uren Verantwoording\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760" activeTab="1"/>
   </bookViews>
@@ -12,12 +17,12 @@
     <sheet name="Uren Roel Meijns" sheetId="3" r:id="rId3"/>
     <sheet name="Uren Jorrit Verheul" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -122,6 +127,15 @@
   </si>
   <si>
     <t>Met menno wat overlegd over de normalisatie.</t>
+  </si>
+  <si>
+    <t>kerntaak 1 afwerken, planning maken kertaak 2 en volgende week. Examen engels (2uur) voor bereiden</t>
+  </si>
+  <si>
+    <t>Normaliseren</t>
+  </si>
+  <si>
+    <t>Normaliseren en opstart test database</t>
   </si>
 </sst>
 </file>
@@ -598,8 +612,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -643,9 +657,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -683,9 +697,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -720,7 +734,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,7 +769,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1609,7 +1623,7 @@
   <dimension ref="B2:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B42" sqref="B18:B42"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1781,17 +1795,21 @@
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" ht="36" x14ac:dyDescent="0.2">
       <c r="B16" s="45" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="56">
         <v>42775</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="41">
+        <v>5</v>
+      </c>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
-      <c r="G16" s="65"/>
+      <c r="G16" s="65" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
     </row>
@@ -1818,7 +1836,7 @@
       <c r="C18" s="42"/>
       <c r="D18" s="43">
         <f>SUM(D13:D17)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E18" s="43">
         <f>SUM(E13:E17)</f>
@@ -1839,10 +1857,14 @@
       <c r="C19" s="56">
         <v>42779</v>
       </c>
-      <c r="D19" s="39"/>
+      <c r="D19" s="39">
+        <v>6</v>
+      </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="64"/>
+      <c r="G19" s="64" t="s">
+        <v>36</v>
+      </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
     </row>
@@ -1853,10 +1875,14 @@
       <c r="C20" s="56">
         <v>42780</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="41">
+        <v>5</v>
+      </c>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="65"/>
+      <c r="G20" s="65" t="s">
+        <v>37</v>
+      </c>
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
@@ -1909,7 +1935,7 @@
       <c r="C24" s="42"/>
       <c r="D24" s="43">
         <f>SUM(D19:D23)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E24" s="43"/>
       <c r="F24" s="43">
@@ -2191,7 +2217,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="36">

</xml_diff>

<commit_message>
Uren ingevuld van woensdag 15-02-2017
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menno\Documents\Wijkertoren-docs\Uren Verantwoording\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Uren Jeffrey Meyer" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="Uren Roel Meijns" sheetId="3" r:id="rId3"/>
     <sheet name="Uren Jorrit Verheul" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="39">
   <si>
     <t>Datum</t>
   </si>
@@ -136,6 +131,9 @@
   </si>
   <si>
     <t>Normaliseren en opstart test database</t>
+  </si>
+  <si>
+    <t>Normalisatie gedaan met menno en database opzetten en engelse toetsen gemaakt morgen bootrap op test databse gooien</t>
   </si>
 </sst>
 </file>
@@ -612,8 +610,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -657,9 +655,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -697,9 +695,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -734,7 +732,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,7 +767,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -945,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1209,17 +1207,21 @@
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B21" s="45" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="56">
         <v>42781</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="41">
+        <v>4</v>
+      </c>
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
-      <c r="G21" s="59"/>
+      <c r="G21" s="59" t="s">
+        <v>38</v>
+      </c>
       <c r="H21" s="27"/>
       <c r="I21" s="18"/>
     </row>
@@ -1258,7 +1260,7 @@
       <c r="C24" s="42"/>
       <c r="D24" s="43">
         <f>SUM(D19:D23)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E24" s="43"/>
       <c r="F24" s="43">
@@ -1510,7 +1512,7 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="36">
@@ -1622,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uren verantwoording ingevuld Jeffrey
Uren verantwoording ingevuld van de week voor de vakantie.
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -137,6 +137,24 @@
   </si>
   <si>
     <t>Database en normalisatie is goed en ontwikkelings omgeving opnieuw ingesteld gekoppeld met Xamp, github en Netbeans. Getest of je branches en issues kan aanmaken en merge met success we gaan er vanuit dat er geen merge conflicts komen en mocht deze voorkomen dan weet ik hoe deze moet worden opgelost.</t>
+  </si>
+  <si>
+    <t>Database genormaliseerd en uitzoeken hoe we de extensie van de website gaan maken.</t>
+  </si>
+  <si>
+    <t>Opzoek naar een manier om de leden overzichtelijk te implementeren of alternatieve manier om dit voor elkaar te krijgen.</t>
+  </si>
+  <si>
+    <t>Menno heeft een plugin van bootstrap gevonden om een data tabel te maken dat wij kunnen gebruiken om alle leden in te laten zien en sorteren op naam, oraganisatie, woonplaats enz.</t>
+  </si>
+  <si>
+    <t>Ziek.</t>
+  </si>
+  <si>
+    <t>Uitgezocht hoe de plugin werkt en hoe je de data uit het database kan halen.</t>
+  </si>
+  <si>
+    <t>Tabellen werken nu wij zijn nu bezig om een manier te vinden hoe we de data op de juiste plekken kunnen implementeren.</t>
   </si>
 </sst>
 </file>
@@ -214,7 +232,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -292,19 +310,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
@@ -410,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -515,48 +520,45 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -569,10 +571,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -584,16 +586,16 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -946,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1013,7 +1015,7 @@
     </row>
     <row r="8" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31"/>
-      <c r="C8" s="54"/>
+      <c r="C8" s="53"/>
       <c r="F8" s="29"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1047,138 +1049,138 @@
       <c r="F11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="47" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="2:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="49"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="26"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="2:9" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="55">
         <v>42772</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="61">
         <v>6</v>
       </c>
-      <c r="E13" s="62"/>
+      <c r="E13" s="61"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="57" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="2:9" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="55">
         <v>42773</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="62">
         <v>4</v>
       </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="59" t="s">
+      <c r="E14" s="62"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="58" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="2:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="55">
         <v>42774</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="62">
         <v>4</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="59" t="s">
+      <c r="E15" s="62"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="58" t="s">
         <v>28</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="55">
         <v>42775</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="62">
         <v>5</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="65" t="s">
+      <c r="E16" s="62"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="64" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
     </row>
     <row r="17" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="55">
         <v>42776</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63">
+      <c r="D17" s="62"/>
+      <c r="E17" s="62">
         <v>7</v>
       </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="51"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="27"/>
       <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43">
+      <c r="C18" s="41"/>
+      <c r="D18" s="42">
         <f>SUM(D13:D17)</f>
         <v>19</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="42">
         <f>SUM(E13:E17)</f>
         <v>7</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="42">
         <f>SUM(F13:F17)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="28"/>
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="55">
         <v>42779</v>
       </c>
       <c r="D19" s="39">
@@ -1186,329 +1188,369 @@
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="57" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="55">
         <v>42780</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="40">
         <v>4</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="59" t="s">
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="58" t="s">
         <v>34</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="55">
         <v>42781</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="40">
         <v>4</v>
       </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="59" t="s">
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="58" t="s">
         <v>38</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="2:9" ht="120" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="56">
+      <c r="C22" s="55">
         <v>42782</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="40">
         <v>7</v>
       </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="59" t="s">
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="58" t="s">
         <v>39</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="45" t="s">
+    <row r="23" spans="2:9" ht="36" x14ac:dyDescent="0.2">
+      <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="56">
+      <c r="C23" s="55">
         <v>42783</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="59"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="58" t="s">
+        <v>40</v>
+      </c>
       <c r="H23" s="27"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43">
+      <c r="C24" s="41"/>
+      <c r="D24" s="42">
         <f>SUM(D19:D23)</f>
         <v>22</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43">
+      <c r="E24" s="42"/>
+      <c r="F24" s="42">
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="28"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="47" t="s">
+    <row r="25" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="39"/>
+      <c r="C25" s="55">
+        <v>42793</v>
+      </c>
+      <c r="D25" s="39">
+        <v>7</v>
+      </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="50"/>
+      <c r="G25" s="57" t="s">
+        <v>41</v>
+      </c>
       <c r="H25" s="27"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="45" t="s">
+    <row r="26" spans="2:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="51"/>
+      <c r="C26" s="55">
+        <v>42794</v>
+      </c>
+      <c r="D26" s="40">
+        <v>4</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="H26" s="27"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="45" t="s">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="51"/>
+      <c r="C27" s="55">
+        <v>42795</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40">
+        <v>4</v>
+      </c>
+      <c r="G27" s="58" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="27"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="45" t="s">
+    <row r="28" spans="2:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="51"/>
+      <c r="C28" s="55">
+        <v>42796</v>
+      </c>
+      <c r="D28" s="40">
+        <v>7</v>
+      </c>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="58" t="s">
+        <v>44</v>
+      </c>
       <c r="H28" s="27"/>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="45" t="s">
+    <row r="29" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="51"/>
+      <c r="C29" s="55">
+        <v>42797</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="H29" s="27"/>
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="43">
+      <c r="C30" s="55"/>
+      <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43">
+        <v>18</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42">
         <f>SUM(F25:F29)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="52"/>
+        <v>4</v>
+      </c>
+      <c r="G30" s="51"/>
       <c r="H30" s="28"/>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="C31" s="55">
+        <v>42800</v>
+      </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="50"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="27"/>
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="51"/>
+      <c r="C32" s="55">
+        <v>42801</v>
+      </c>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="50"/>
       <c r="H32" s="27"/>
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="51"/>
+      <c r="C33" s="55">
+        <v>42802</v>
+      </c>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="27"/>
       <c r="I33" s="18"/>
     </row>
     <row r="34" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="51"/>
+      <c r="C34" s="55">
+        <v>42803</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="27"/>
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="51"/>
+      <c r="C35" s="55">
+        <v>42804</v>
+      </c>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="27"/>
       <c r="I35" s="18"/>
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43">
+      <c r="C36" s="41"/>
+      <c r="D36" s="42">
         <f>SUM(D31:D35)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43">
+      <c r="E36" s="42"/>
+      <c r="F36" s="42">
         <f>SUM(F31:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="28"/>
       <c r="I36" s="19"/>
     </row>
     <row r="37" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="56"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="50"/>
+      <c r="G37" s="49"/>
       <c r="H37" s="27"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="51"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="50"/>
       <c r="H38" s="27"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="51"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="27"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="51"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="27"/>
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="51"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43">
+      <c r="C42" s="41"/>
+      <c r="D42" s="42">
         <f>SUM(D37:D41)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43">
+      <c r="E42" s="42"/>
+      <c r="F42" s="42">
         <f>SUM(F37:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="52"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
@@ -1519,14 +1561,14 @@
       </c>
       <c r="D43" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="36">
         <f>SUM(F18+F24+F30+F36+F42)</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="G43" s="52"/>
       <c r="H43" s="27"/>
       <c r="I43" s="4"/>
     </row>
@@ -1550,13 +1592,13 @@
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="69"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="33"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="57" t="s">
+      <c r="E46" s="66"/>
+      <c r="F46" s="56" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="21"/>
@@ -1631,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -1641,8 +1683,8 @@
     <col min="2" max="2" width="13.42578125" style="23"/>
     <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
-    <col min="7" max="7" width="33" style="54" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="54" customWidth="1"/>
+    <col min="7" max="7" width="33" style="53" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="53" customWidth="1"/>
     <col min="9" max="16384" width="13.42578125" style="13"/>
   </cols>
   <sheetData>
@@ -1698,7 +1740,7 @@
     </row>
     <row r="8" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31"/>
-      <c r="C8" s="54"/>
+      <c r="C8" s="53"/>
       <c r="F8" s="29"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1732,29 +1774,29 @@
       <c r="F11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="47" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="2:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="49"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="26"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="2:9" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="55">
         <v>42772</v>
       </c>
       <c r="D13" s="39">
@@ -1762,108 +1804,108 @@
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="63" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="55">
         <v>42773</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="40">
         <v>4</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="65" t="s">
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="64" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="2:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="55">
         <v>42774</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="40">
         <v>4</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="65" t="s">
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="64" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="55">
         <v>42775</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="40">
         <v>5</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="65" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="64" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
     </row>
     <row r="17" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="55">
         <v>42776</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40">
         <v>7</v>
       </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="65"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="27"/>
       <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43">
+      <c r="C18" s="41"/>
+      <c r="D18" s="42">
         <f>SUM(D13:D17)</f>
         <v>19</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="42">
         <f>SUM(E13:E17)</f>
         <v>7</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="42">
         <f>SUM(F13:F17)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="66"/>
+      <c r="G18" s="65"/>
       <c r="H18" s="28"/>
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="55">
         <v>42779</v>
       </c>
       <c r="D19" s="39">
@@ -1871,351 +1913,351 @@
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="64" t="s">
+      <c r="G19" s="63" t="s">
         <v>36</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="55">
         <v>42780</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="40">
         <v>5</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="65" t="s">
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="64" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="55">
         <v>42781</v>
       </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="65"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="27"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="56">
+      <c r="C22" s="55">
         <v>42782</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="65"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="27"/>
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="56">
+      <c r="C23" s="55">
         <v>42783</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="65"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="27"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43">
+      <c r="C24" s="41"/>
+      <c r="D24" s="42">
         <f>SUM(D19:D23)</f>
         <v>11</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43">
+      <c r="E24" s="42"/>
+      <c r="F24" s="42">
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="66"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="28"/>
       <c r="I24" s="19"/>
     </row>
     <row r="25" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="56">
+      <c r="C25" s="55">
         <v>42786</v>
       </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="64"/>
+      <c r="G25" s="63"/>
       <c r="H25" s="27"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="55">
         <v>42787</v>
       </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="65"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="64"/>
       <c r="H26" s="27"/>
       <c r="I26" s="18"/>
     </row>
     <row r="27" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="56">
+      <c r="C27" s="55">
         <v>42788</v>
       </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="65"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="27"/>
       <c r="I27" s="18"/>
     </row>
     <row r="28" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="56">
+      <c r="C28" s="55">
         <v>42789</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="65"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="64"/>
       <c r="H28" s="27"/>
       <c r="I28" s="18"/>
     </row>
     <row r="29" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="55">
         <v>42790</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="65"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="27"/>
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43">
+      <c r="C30" s="41"/>
+      <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43">
+      <c r="E30" s="42"/>
+      <c r="F30" s="42">
         <f>SUM(F25:F29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="66"/>
+      <c r="G30" s="65"/>
       <c r="H30" s="28"/>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="56">
+      <c r="C31" s="55">
         <v>42793</v>
       </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="64"/>
+      <c r="G31" s="63"/>
       <c r="H31" s="27"/>
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="56">
+      <c r="C32" s="55">
         <v>42794</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="65"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="27"/>
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="56">
+      <c r="C33" s="55">
         <v>42795</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="65"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="27"/>
       <c r="I33" s="18"/>
     </row>
     <row r="34" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="56">
+      <c r="C34" s="55">
         <v>42796</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="65"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="27"/>
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="56">
+      <c r="C35" s="55">
         <v>42797</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="65"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="27"/>
       <c r="I35" s="18"/>
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43">
+      <c r="C36" s="41"/>
+      <c r="D36" s="42">
         <f>SUM(D31:D35)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43">
+      <c r="E36" s="42"/>
+      <c r="F36" s="42">
         <f>SUM(F31:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="66"/>
+      <c r="G36" s="65"/>
       <c r="H36" s="28"/>
       <c r="I36" s="19"/>
     </row>
     <row r="37" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="56">
+      <c r="C37" s="55">
         <v>42800</v>
       </c>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="64"/>
+      <c r="G37" s="63"/>
       <c r="H37" s="27"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="56">
+      <c r="C38" s="55">
         <v>42801</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="65"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="27"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="56">
+      <c r="C39" s="55">
         <v>42802</v>
       </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="65"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="27"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="56">
+      <c r="C40" s="55">
         <v>42803</v>
       </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="65"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="27"/>
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="56">
+      <c r="C41" s="55">
         <v>42804</v>
       </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="65"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43">
+      <c r="C42" s="41"/>
+      <c r="D42" s="42">
         <f>SUM(D37:D41)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43">
+      <c r="E42" s="42"/>
+      <c r="F42" s="42">
         <f>SUM(F37:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="66"/>
+      <c r="G42" s="65"/>
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
@@ -2233,7 +2275,7 @@
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="52"/>
       <c r="H43" s="27"/>
       <c r="I43" s="4"/>
     </row>
@@ -2257,13 +2299,13 @@
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="60" t="s">
+      <c r="C46" s="68"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="59" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="21"/>
@@ -2338,8 +2380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2348,8 +2390,8 @@
     <col min="2" max="2" width="13.42578125" style="23"/>
     <col min="3" max="3" width="11.7109375" style="13" customWidth="1"/>
     <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
-    <col min="7" max="7" width="33" style="54" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="54" customWidth="1"/>
+    <col min="7" max="7" width="33" style="53" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="53" customWidth="1"/>
     <col min="9" max="16384" width="13.42578125" style="13"/>
   </cols>
   <sheetData>
@@ -2405,7 +2447,7 @@
     </row>
     <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31"/>
-      <c r="C8" s="54"/>
+      <c r="C8" s="53"/>
       <c r="F8" s="29"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2439,29 +2481,29 @@
       <c r="F11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="47" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="49"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="26"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" s="16" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="55">
         <v>42772</v>
       </c>
       <c r="D13" s="39">
@@ -2469,7 +2511,7 @@
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="57" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="27"/>
@@ -2477,405 +2519,425 @@
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="55">
         <v>42773</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40">
         <v>5</v>
       </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="51"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="27"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="55">
         <v>42774</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="40">
         <v>4</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="59" t="s">
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="58" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="55">
         <v>42775</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="40">
         <v>4</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="59" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="58" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
     </row>
     <row r="17" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="55">
         <v>42776</v>
       </c>
-      <c r="D17" s="41">
+      <c r="D17" s="40">
         <v>3</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="59" t="s">
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="58" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43">
+      <c r="C18" s="41"/>
+      <c r="D18" s="42">
         <f>SUM(D13:D17)</f>
         <v>14</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="42">
         <f>SUM(E13:E17)</f>
         <v>5</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="42">
         <f>SUM(F13:F17)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="28"/>
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="56"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="50"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="51"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="50"/>
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="27"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="51"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="27"/>
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="51"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="27"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43">
+      <c r="C24" s="41"/>
+      <c r="D24" s="42">
         <f>SUM(D19:D23)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43">
+      <c r="E24" s="42"/>
+      <c r="F24" s="42">
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="28"/>
       <c r="I24" s="19"/>
     </row>
     <row r="25" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="56"/>
+      <c r="C25" s="55">
+        <v>42793</v>
+      </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="50"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="27"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="51"/>
+      <c r="C26" s="55">
+        <v>42794</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="27"/>
       <c r="I26" s="18"/>
     </row>
     <row r="27" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="51"/>
+      <c r="C27" s="55">
+        <v>42795</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="50"/>
       <c r="H27" s="27"/>
       <c r="I27" s="18"/>
     </row>
     <row r="28" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="51"/>
+      <c r="C28" s="55">
+        <v>42796</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="27"/>
       <c r="I28" s="18"/>
     </row>
     <row r="29" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="51"/>
+      <c r="C29" s="55">
+        <v>42797</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="50"/>
       <c r="H29" s="27"/>
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="43">
+      <c r="C30" s="55"/>
+      <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43">
+      <c r="E30" s="42"/>
+      <c r="F30" s="42">
         <f>SUM(F25:F29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="28"/>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="C31" s="55">
+        <v>42800</v>
+      </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="50"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="27"/>
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="51"/>
+      <c r="C32" s="55">
+        <v>42801</v>
+      </c>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="50"/>
       <c r="H32" s="27"/>
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="51"/>
+      <c r="C33" s="55">
+        <v>42802</v>
+      </c>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="27"/>
       <c r="I33" s="18"/>
     </row>
     <row r="34" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="51"/>
+      <c r="C34" s="55">
+        <v>42803</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="27"/>
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="51"/>
+      <c r="C35" s="55">
+        <v>42804</v>
+      </c>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="27"/>
       <c r="I35" s="18"/>
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43">
+      <c r="C36" s="41"/>
+      <c r="D36" s="42">
         <f>SUM(D31:D35)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43">
+      <c r="E36" s="42"/>
+      <c r="F36" s="42">
         <f>SUM(F31:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="28"/>
       <c r="I36" s="19"/>
     </row>
     <row r="37" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="56"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="50"/>
+      <c r="G37" s="49"/>
       <c r="H37" s="27"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="51"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="50"/>
       <c r="H38" s="27"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="51"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="27"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="51"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="27"/>
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="51"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43">
+      <c r="C42" s="41"/>
+      <c r="D42" s="42">
         <f>SUM(D37:D41)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43">
+      <c r="E42" s="42"/>
+      <c r="F42" s="42">
         <f>SUM(F37:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="52"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
@@ -2893,7 +2955,7 @@
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="52"/>
       <c r="H43" s="27"/>
       <c r="I43" s="4"/>
     </row>
@@ -2917,13 +2979,13 @@
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="60" t="s">
+      <c r="C46" s="68"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="59" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="21"/>
@@ -2997,18 +3059,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="23"/>
-    <col min="3" max="3" width="8.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
-    <col min="7" max="7" width="33" style="54" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="54" customWidth="1"/>
+    <col min="7" max="7" width="33" style="53" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="53" customWidth="1"/>
     <col min="9" max="16384" width="13.42578125" style="13"/>
   </cols>
   <sheetData>
@@ -3064,7 +3126,7 @@
     </row>
     <row r="8" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31"/>
-      <c r="C8" s="54"/>
+      <c r="C8" s="53"/>
       <c r="F8" s="29"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -3098,29 +3160,29 @@
       <c r="F11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="47" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="2:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="49"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="26"/>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="2:9" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="61">
+      <c r="C13" s="60">
         <v>42772</v>
       </c>
       <c r="D13" s="39">
@@ -3128,438 +3190,428 @@
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="49" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="2:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="61">
+      <c r="C14" s="60">
         <v>42773</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="51"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="27"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="61">
+      <c r="C15" s="60">
         <v>42774</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="51"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="27"/>
       <c r="I15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="61">
+      <c r="C16" s="60">
         <v>42775</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="51"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="50"/>
       <c r="H16" s="27"/>
       <c r="I16" s="18"/>
     </row>
     <row r="17" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="61">
+      <c r="C17" s="60">
         <v>42776</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="51"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="27"/>
       <c r="I17" s="18"/>
     </row>
     <row r="18" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43">
+      <c r="C18" s="41"/>
+      <c r="D18" s="42">
         <f>SUM(D13:D17)</f>
         <v>5</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="42">
         <f>SUM(E13:E17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="42">
         <f>SUM(F13:F17)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="28"/>
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="61">
+      <c r="C19" s="60">
         <v>42779</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="50"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="27"/>
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="61">
+      <c r="C20" s="60">
         <v>42780</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="51"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="50"/>
       <c r="H20" s="27"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="61">
+      <c r="C21" s="60">
         <v>42781</v>
       </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="51"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="27"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="61">
+      <c r="C22" s="60">
         <v>42782</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="51"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="27"/>
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="61">
+      <c r="C23" s="60">
         <v>42783</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="51"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="27"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43">
+      <c r="C24" s="41"/>
+      <c r="D24" s="42">
         <f>SUM(D19:D23)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43">
+      <c r="E24" s="42"/>
+      <c r="F24" s="42">
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="28"/>
       <c r="I24" s="19"/>
     </row>
     <row r="25" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="61">
-        <v>42786</v>
+      <c r="C25" s="55">
+        <v>42793</v>
       </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="50"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="27"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="61">
-        <v>42787</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="51"/>
+      <c r="C26" s="55">
+        <v>42794</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="27"/>
       <c r="I26" s="18"/>
     </row>
     <row r="27" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="61">
-        <v>42788</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="51"/>
+      <c r="C27" s="55">
+        <v>42795</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="50"/>
       <c r="H27" s="27"/>
       <c r="I27" s="18"/>
     </row>
     <row r="28" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="61">
-        <v>42789</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="51"/>
+      <c r="C28" s="55">
+        <v>42796</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="27"/>
       <c r="I28" s="18"/>
     </row>
     <row r="29" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="61">
-        <v>42790</v>
-      </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="51"/>
+      <c r="C29" s="55">
+        <v>42797</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="50"/>
       <c r="H29" s="27"/>
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="43">
+      <c r="C30" s="55"/>
+      <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43">
+      <c r="E30" s="42"/>
+      <c r="F30" s="42">
         <f>SUM(F25:F29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="28"/>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="61">
-        <v>42793</v>
+      <c r="C31" s="55">
+        <v>42800</v>
       </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="50"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="27"/>
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="61">
-        <v>42794</v>
-      </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="51"/>
+      <c r="C32" s="55">
+        <v>42801</v>
+      </c>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="50"/>
       <c r="H32" s="27"/>
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="61">
-        <v>42795</v>
-      </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="51"/>
+      <c r="C33" s="55">
+        <v>42802</v>
+      </c>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="27"/>
       <c r="I33" s="18"/>
     </row>
     <row r="34" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="61">
-        <v>42796</v>
-      </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="51"/>
+      <c r="C34" s="55">
+        <v>42803</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="27"/>
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="61">
-        <v>42797</v>
-      </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="51"/>
+      <c r="C35" s="55">
+        <v>42804</v>
+      </c>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="27"/>
       <c r="I35" s="18"/>
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="43">
+      <c r="C36" s="41"/>
+      <c r="D36" s="42">
         <f>SUM(D31:D35)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43">
+      <c r="E36" s="42"/>
+      <c r="F36" s="42">
         <f>SUM(F31:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="28"/>
       <c r="I36" s="19"/>
     </row>
     <row r="37" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="61">
-        <v>42889</v>
-      </c>
+      <c r="C37" s="60"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="50"/>
+      <c r="G37" s="49"/>
       <c r="H37" s="27"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="61">
-        <v>42890</v>
-      </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="51"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="50"/>
       <c r="H38" s="27"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="61">
-        <v>42891</v>
-      </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="51"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="50"/>
       <c r="H39" s="27"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="61">
-        <v>42892</v>
-      </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="51"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="27"/>
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="61">
-        <v>42893</v>
-      </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="51"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43">
+      <c r="C42" s="41"/>
+      <c r="D42" s="42">
         <f>SUM(D37:D41)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43">
+      <c r="E42" s="42"/>
+      <c r="F42" s="42">
         <f>SUM(F37:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="52"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
@@ -3577,7 +3629,7 @@
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="53"/>
+      <c r="G43" s="52"/>
       <c r="H43" s="27"/>
       <c r="I43" s="4"/>
     </row>
@@ -3601,13 +3653,13 @@
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="60" t="s">
+      <c r="C46" s="68"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="59" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="21"/>

</xml_diff>

<commit_message>
Uren verantwoording ingevuld :D
WOOP WOOP
</commit_message>
<xml_diff>
--- a/Uren Verantwoording/Uren Verantwoording.xlsx
+++ b/Uren Verantwoording/Uren Verantwoording.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKSPACE\Wijkertoren\Wijkertoren-docs\Uren Verantwoording\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="18972" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Uren Jeffrey Meyer" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="Uren Roel Meijns" sheetId="3" r:id="rId3"/>
     <sheet name="Uren Jorrit Verheul" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -175,6 +170,39 @@
   </si>
   <si>
     <t>Documentatie</t>
+  </si>
+  <si>
+    <t>Vrijdag / Zaterdag</t>
+  </si>
+  <si>
+    <t>Data staat de goed manier in de tabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemen gekregen met de tabel we moeten een andere manier zien te vinden de data op de tabel te krijgen. </t>
+  </si>
+  <si>
+    <t>plan uitbedacht hoe we de data juist kunnen krijgen en deze morge in werking zetten.</t>
+  </si>
+  <si>
+    <t>Tabel is nu goed met alle elementen die erin moeten staan nu bedenken samen met Menno hoe we de buttons gaan doen en waar deze nog moeten komen te staan.</t>
+  </si>
+  <si>
+    <t>Ik ben bezig met het maken voor de modal (pop-up) om de informatie te laten weergeven is niet al te moeilijk hoop ik.</t>
+  </si>
+  <si>
+    <t>Modals maken ging lastiger dan dat ik had gedacht heb ze nu wel gemaakt.</t>
+  </si>
+  <si>
+    <t>Nu ben ik bezig met menno de functionaliteit te maken voor de buttons alle elementen voor een lid toetevoegen staan al in de modal moeten alleen nog via jQuery en ajax deze gegevens door kunnen sturen naar de database om ze toe te voegen.</t>
+  </si>
+  <si>
+    <t>Websites door kijken hoe ik data kan laten opslaan in de database.</t>
+  </si>
+  <si>
+    <t>In mijn vrije tijd even doorkijken hoe ik de data moet doorsturen en ophalen van de database.</t>
+  </si>
+  <si>
+    <t>17-3-2017 18-3-2017</t>
   </si>
 </sst>
 </file>
@@ -582,44 +610,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -722,7 +750,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,7 +785,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -968,22 +996,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="23"/>
-    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.88671875" style="13" customWidth="1"/>
     <col min="7" max="7" width="33" style="22" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="13.42578125" style="13"/>
+    <col min="8" max="8" width="10.5546875" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="13.44140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
@@ -994,7 +1022,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1003,7 +1031,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
         <v>15</v>
       </c>
@@ -1019,7 +1047,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="1"/>
       <c r="F6" s="32"/>
@@ -1040,7 +1068,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1091,15 +1119,15 @@
       <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="54">
         <v>42772</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="59">
         <v>6</v>
       </c>
-      <c r="E13" s="61"/>
+      <c r="E13" s="59"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="56" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="27"/>
@@ -1109,15 +1137,15 @@
       <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="54">
         <v>42773</v>
       </c>
-      <c r="D14" s="62">
+      <c r="D14" s="60">
         <v>4</v>
       </c>
-      <c r="E14" s="62"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="40"/>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="57" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="27"/>
@@ -1127,15 +1155,15 @@
       <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="55">
+      <c r="C15" s="54">
         <v>42774</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="60">
         <v>4</v>
       </c>
-      <c r="E15" s="62"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="40"/>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="57" t="s">
         <v>28</v>
       </c>
       <c r="H15" s="27"/>
@@ -1145,15 +1173,15 @@
       <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="54">
         <v>42775</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="60">
         <v>5</v>
       </c>
-      <c r="E16" s="62"/>
+      <c r="E16" s="60"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="64" t="s">
+      <c r="G16" s="62" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="27"/>
@@ -1163,11 +1191,11 @@
       <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="55">
+      <c r="C17" s="54">
         <v>42776</v>
       </c>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62">
+      <c r="D17" s="60"/>
+      <c r="E17" s="60">
         <v>7</v>
       </c>
       <c r="F17" s="40"/>
@@ -1200,7 +1228,7 @@
       <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="55">
+      <c r="C19" s="54">
         <v>42779</v>
       </c>
       <c r="D19" s="39">
@@ -1208,7 +1236,7 @@
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="56" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="27"/>
@@ -1218,7 +1246,7 @@
       <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="54">
         <v>42780</v>
       </c>
       <c r="D20" s="40">
@@ -1226,7 +1254,7 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="57" t="s">
         <v>34</v>
       </c>
       <c r="H20" s="27"/>
@@ -1236,7 +1264,7 @@
       <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="55">
+      <c r="C21" s="54">
         <v>42781</v>
       </c>
       <c r="D21" s="40">
@@ -1244,7 +1272,7 @@
       </c>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
-      <c r="G21" s="58" t="s">
+      <c r="G21" s="57" t="s">
         <v>38</v>
       </c>
       <c r="H21" s="27"/>
@@ -1254,7 +1282,7 @@
       <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="54">
         <v>42782</v>
       </c>
       <c r="D22" s="40">
@@ -1262,7 +1290,7 @@
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
-      <c r="G22" s="58" t="s">
+      <c r="G22" s="57" t="s">
         <v>39</v>
       </c>
       <c r="H22" s="27"/>
@@ -1272,13 +1300,13 @@
       <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="55">
+      <c r="C23" s="54">
         <v>42783</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="57" t="s">
         <v>40</v>
       </c>
       <c r="H23" s="27"/>
@@ -1306,7 +1334,7 @@
       <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="55">
+      <c r="C25" s="54">
         <v>42793</v>
       </c>
       <c r="D25" s="39">
@@ -1314,7 +1342,7 @@
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="56" t="s">
         <v>41</v>
       </c>
       <c r="H25" s="27"/>
@@ -1324,7 +1352,7 @@
       <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="54">
         <v>42794</v>
       </c>
       <c r="D26" s="40">
@@ -1332,17 +1360,17 @@
       </c>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="57" t="s">
         <v>42</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="54">
         <v>42795</v>
       </c>
       <c r="D27" s="40"/>
@@ -1350,7 +1378,7 @@
       <c r="F27" s="40">
         <v>4</v>
       </c>
-      <c r="G27" s="58" t="s">
+      <c r="G27" s="57" t="s">
         <v>43</v>
       </c>
       <c r="H27" s="27"/>
@@ -1360,7 +1388,7 @@
       <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="54">
         <v>42796</v>
       </c>
       <c r="D28" s="40">
@@ -1368,7 +1396,7 @@
       </c>
       <c r="E28" s="40"/>
       <c r="F28" s="40"/>
-      <c r="G28" s="58" t="s">
+      <c r="G28" s="57" t="s">
         <v>44</v>
       </c>
       <c r="H28" s="27"/>
@@ -1378,13 +1406,13 @@
       <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="54">
         <v>42797</v>
       </c>
       <c r="D29" s="40"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
-      <c r="G29" s="58" t="s">
+      <c r="G29" s="57" t="s">
         <v>45</v>
       </c>
       <c r="H29" s="27"/>
@@ -1394,7 +1422,7 @@
       <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="55"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
         <v>18</v>
@@ -1412,55 +1440,71 @@
       <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="55">
+      <c r="C31" s="54">
         <v>42800</v>
       </c>
-      <c r="D31" s="39"/>
+      <c r="D31" s="39">
+        <v>7</v>
+      </c>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="49"/>
+      <c r="G31" s="49" t="s">
+        <v>52</v>
+      </c>
       <c r="H31" s="27"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" ht="34.200000000000003" x14ac:dyDescent="0.2">
       <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="54">
         <v>42801</v>
       </c>
-      <c r="D32" s="40"/>
+      <c r="D32" s="40">
+        <v>4</v>
+      </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
-      <c r="G32" s="50"/>
+      <c r="G32" s="57" t="s">
+        <v>53</v>
+      </c>
       <c r="H32" s="27"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" ht="34.200000000000003" x14ac:dyDescent="0.2">
       <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="55">
+      <c r="C33" s="54">
         <v>42802</v>
       </c>
-      <c r="D33" s="40"/>
+      <c r="D33" s="40">
+        <v>4</v>
+      </c>
       <c r="E33" s="40"/>
       <c r="F33" s="40"/>
-      <c r="G33" s="50"/>
+      <c r="G33" s="57" t="s">
+        <v>54</v>
+      </c>
       <c r="H33" s="27"/>
       <c r="I33" s="18"/>
     </row>
-    <row r="34" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" ht="57" x14ac:dyDescent="0.2">
       <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <v>42803</v>
       </c>
-      <c r="D34" s="40"/>
+      <c r="D34" s="40">
+        <v>7</v>
+      </c>
       <c r="E34" s="40"/>
       <c r="F34" s="40"/>
-      <c r="G34" s="50"/>
+      <c r="G34" s="57" t="s">
+        <v>55</v>
+      </c>
       <c r="H34" s="27"/>
       <c r="I34" s="18"/>
     </row>
@@ -1468,7 +1512,7 @@
       <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="55">
+      <c r="C35" s="54">
         <v>42804</v>
       </c>
       <c r="D35" s="40"/>
@@ -1478,14 +1522,14 @@
       <c r="H35" s="27"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="41"/>
       <c r="D36" s="42">
         <f>SUM(D31:D35)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E36" s="42"/>
       <c r="F36" s="42">
@@ -1496,74 +1540,104 @@
       <c r="H36" s="28"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" ht="34.200000000000003" x14ac:dyDescent="0.2">
       <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="39"/>
+      <c r="C37" s="54">
+        <v>42807</v>
+      </c>
+      <c r="D37" s="39">
+        <v>7</v>
+      </c>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="49"/>
+      <c r="G37" s="56" t="s">
+        <v>56</v>
+      </c>
       <c r="H37" s="27"/>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" ht="22.8" x14ac:dyDescent="0.2">
       <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="40"/>
+      <c r="C38" s="54">
+        <v>42808</v>
+      </c>
+      <c r="D38" s="40">
+        <v>4</v>
+      </c>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
-      <c r="G38" s="50"/>
+      <c r="G38" s="57" t="s">
+        <v>57</v>
+      </c>
       <c r="H38" s="27"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" ht="79.8" x14ac:dyDescent="0.2">
       <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="40"/>
+      <c r="C39" s="54">
+        <v>42809</v>
+      </c>
+      <c r="D39" s="40">
+        <v>4</v>
+      </c>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
-      <c r="G39" s="50"/>
+      <c r="G39" s="57" t="s">
+        <v>58</v>
+      </c>
       <c r="H39" s="27"/>
       <c r="I39" s="18"/>
     </row>
-    <row r="40" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" ht="22.8" x14ac:dyDescent="0.2">
       <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="40"/>
+      <c r="C40" s="54">
+        <v>42810</v>
+      </c>
+      <c r="D40" s="40">
+        <v>7</v>
+      </c>
       <c r="E40" s="40"/>
       <c r="F40" s="40"/>
-      <c r="G40" s="50"/>
+      <c r="G40" s="57" t="s">
+        <v>59</v>
+      </c>
       <c r="H40" s="27"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" ht="34.200000000000003" x14ac:dyDescent="0.2">
       <c r="B41" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="40">
+        <v>8</v>
+      </c>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
-      <c r="G41" s="50"/>
+      <c r="G41" s="57" t="s">
+        <v>60</v>
+      </c>
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="41"/>
       <c r="D42" s="42">
         <f>SUM(D37:D41)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E42" s="42"/>
       <c r="F42" s="42">
@@ -1574,103 +1648,134 @@
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="35" t="s">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="54">
+        <v>42814</v>
+      </c>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="54">
+        <v>42815</v>
+      </c>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="54">
+        <v>42816</v>
+      </c>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="54">
+        <v>42817</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="54">
+        <v>42818</v>
+      </c>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="2:9" s="14" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42">
+        <f>SUM(D43:D47)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42">
+        <f>SUM(F43:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="51"/>
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="2:8" s="14" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="9"/>
+      <c r="C49" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D49" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
-        <v>59</v>
-      </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36">
+        <v>111</v>
+      </c>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36">
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>4</v>
       </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="9"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="67" t="s">
+      <c r="G49" s="52"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="9"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.25">
+      <c r="B52" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="68"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="56" t="s">
+      <c r="C52" s="68"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="64"/>
+      <c r="F52" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-    </row>
-    <row r="47" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-    </row>
-    <row r="48" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-    </row>
-    <row r="49" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="8"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="8"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="8"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="G52" s="21"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
@@ -1681,7 +1786,7 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B52:C52"/>
     <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.17" top="0.21" bottom="0.16" header="0.25" footer="0.16"/>
@@ -1693,22 +1798,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="23"/>
-    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="23"/>
+    <col min="3" max="3" width="9.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.88671875" style="13" customWidth="1"/>
     <col min="7" max="7" width="33" style="53" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="53" customWidth="1"/>
-    <col min="9" max="16384" width="13.42578125" style="13"/>
+    <col min="8" max="8" width="10.5546875" style="53" customWidth="1"/>
+    <col min="9" max="16384" width="13.44140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
@@ -1719,7 +1824,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1728,7 +1833,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
         <v>16</v>
       </c>
@@ -1744,7 +1849,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="1"/>
       <c r="F6" s="32"/>
@@ -1765,7 +1870,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1816,7 +1921,7 @@
       <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="54">
         <v>42772</v>
       </c>
       <c r="D13" s="39">
@@ -1824,17 +1929,17 @@
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="63" t="s">
+      <c r="G13" s="61" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="54">
         <v>42773</v>
       </c>
       <c r="D14" s="40">
@@ -1842,7 +1947,7 @@
       </c>
       <c r="E14" s="40"/>
       <c r="F14" s="40"/>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="62" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="27"/>
@@ -1852,7 +1957,7 @@
       <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="55">
+      <c r="C15" s="54">
         <v>42774</v>
       </c>
       <c r="D15" s="40">
@@ -1860,7 +1965,7 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
-      <c r="G15" s="64" t="s">
+      <c r="G15" s="62" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="27"/>
@@ -1870,7 +1975,7 @@
       <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="54">
         <v>42775</v>
       </c>
       <c r="D16" s="40">
@@ -1878,7 +1983,7 @@
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="64" t="s">
+      <c r="G16" s="62" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="27"/>
@@ -1888,7 +1993,7 @@
       <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="55">
+      <c r="C17" s="54">
         <v>42776</v>
       </c>
       <c r="D17" s="40"/>
@@ -1896,7 +2001,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="40"/>
-      <c r="G17" s="64"/>
+      <c r="G17" s="62"/>
       <c r="H17" s="27"/>
       <c r="I17" s="18"/>
     </row>
@@ -1917,7 +2022,7 @@
         <f>SUM(F13:F17)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="65"/>
+      <c r="G18" s="63"/>
       <c r="H18" s="28"/>
       <c r="I18" s="19"/>
     </row>
@@ -1925,7 +2030,7 @@
       <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="55">
+      <c r="C19" s="54">
         <v>42779</v>
       </c>
       <c r="D19" s="39">
@@ -1933,7 +2038,7 @@
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
-      <c r="G19" s="63" t="s">
+      <c r="G19" s="61" t="s">
         <v>36</v>
       </c>
       <c r="H19" s="27"/>
@@ -1943,7 +2048,7 @@
       <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="54">
         <v>42780</v>
       </c>
       <c r="D20" s="40">
@@ -1951,7 +2056,7 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
-      <c r="G20" s="64" t="s">
+      <c r="G20" s="62" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="27"/>
@@ -1961,13 +2066,13 @@
       <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="55">
+      <c r="C21" s="54">
         <v>42781</v>
       </c>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
-      <c r="G21" s="64"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="27"/>
       <c r="I21" s="18"/>
     </row>
@@ -1975,13 +2080,13 @@
       <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="54">
         <v>42782</v>
       </c>
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
-      <c r="G22" s="64"/>
+      <c r="G22" s="62"/>
       <c r="H22" s="27"/>
       <c r="I22" s="18"/>
     </row>
@@ -1989,13 +2094,13 @@
       <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="55">
+      <c r="C23" s="54">
         <v>42783</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
-      <c r="G23" s="64"/>
+      <c r="G23" s="62"/>
       <c r="H23" s="27"/>
       <c r="I23" s="18"/>
     </row>
@@ -2013,7 +2118,7 @@
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="65"/>
+      <c r="G24" s="63"/>
       <c r="H24" s="28"/>
       <c r="I24" s="19"/>
     </row>
@@ -2021,13 +2126,13 @@
       <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="55">
+      <c r="C25" s="54">
         <v>42786</v>
       </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="63"/>
+      <c r="G25" s="61"/>
       <c r="H25" s="27"/>
       <c r="I25" s="18"/>
     </row>
@@ -2035,13 +2140,13 @@
       <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="54">
         <v>42787</v>
       </c>
       <c r="D26" s="40"/>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
-      <c r="G26" s="64"/>
+      <c r="G26" s="62"/>
       <c r="H26" s="27"/>
       <c r="I26" s="18"/>
     </row>
@@ -2049,13 +2154,13 @@
       <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="54">
         <v>42788</v>
       </c>
       <c r="D27" s="40"/>
       <c r="E27" s="40"/>
       <c r="F27" s="40"/>
-      <c r="G27" s="64"/>
+      <c r="G27" s="62"/>
       <c r="H27" s="27"/>
       <c r="I27" s="18"/>
     </row>
@@ -2063,13 +2168,13 @@
       <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="54">
         <v>42789</v>
       </c>
       <c r="D28" s="40"/>
       <c r="E28" s="40"/>
       <c r="F28" s="40"/>
-      <c r="G28" s="64"/>
+      <c r="G28" s="62"/>
       <c r="H28" s="27"/>
       <c r="I28" s="18"/>
     </row>
@@ -2077,13 +2182,13 @@
       <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="54">
         <v>42790</v>
       </c>
       <c r="D29" s="40"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
-      <c r="G29" s="64"/>
+      <c r="G29" s="62"/>
       <c r="H29" s="27"/>
       <c r="I29" s="18"/>
     </row>
@@ -2101,7 +2206,7 @@
         <f>SUM(F25:F29)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="65"/>
+      <c r="G30" s="63"/>
       <c r="H30" s="28"/>
       <c r="I30" s="19"/>
     </row>
@@ -2109,13 +2214,13 @@
       <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="55">
+      <c r="C31" s="54">
         <v>42793</v>
       </c>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="63"/>
+      <c r="G31" s="61"/>
       <c r="H31" s="27"/>
       <c r="I31" s="18"/>
     </row>
@@ -2123,13 +2228,13 @@
       <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="54">
         <v>42794</v>
       </c>
       <c r="D32" s="40"/>
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
-      <c r="G32" s="64"/>
+      <c r="G32" s="62"/>
       <c r="H32" s="27"/>
       <c r="I32" s="18"/>
     </row>
@@ -2137,13 +2242,13 @@
       <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="55">
+      <c r="C33" s="54">
         <v>42795</v>
       </c>
       <c r="D33" s="40"/>
       <c r="E33" s="40"/>
       <c r="F33" s="40"/>
-      <c r="G33" s="64"/>
+      <c r="G33" s="62"/>
       <c r="H33" s="27"/>
       <c r="I33" s="18"/>
     </row>
@@ -2151,13 +2256,13 @@
       <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <v>42796</v>
       </c>
       <c r="D34" s="40"/>
       <c r="E34" s="40"/>
       <c r="F34" s="40"/>
-      <c r="G34" s="64"/>
+      <c r="G34" s="62"/>
       <c r="H34" s="27"/>
       <c r="I34" s="18"/>
     </row>
@@ -2165,13 +2270,13 @@
       <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="55">
+      <c r="C35" s="54">
         <v>42797</v>
       </c>
       <c r="D35" s="40"/>
       <c r="E35" s="40"/>
       <c r="F35" s="40"/>
-      <c r="G35" s="64"/>
+      <c r="G35" s="62"/>
       <c r="H35" s="27"/>
       <c r="I35" s="18"/>
     </row>
@@ -2189,7 +2294,7 @@
         <f>SUM(F31:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="65"/>
+      <c r="G36" s="63"/>
       <c r="H36" s="28"/>
       <c r="I36" s="19"/>
     </row>
@@ -2197,13 +2302,13 @@
       <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="55">
+      <c r="C37" s="54">
         <v>42800</v>
       </c>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="63"/>
+      <c r="G37" s="61"/>
       <c r="H37" s="27"/>
       <c r="I37" s="18"/>
     </row>
@@ -2211,13 +2316,13 @@
       <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="55">
+      <c r="C38" s="54">
         <v>42801</v>
       </c>
       <c r="D38" s="40"/>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
-      <c r="G38" s="64"/>
+      <c r="G38" s="62"/>
       <c r="H38" s="27"/>
       <c r="I38" s="18"/>
     </row>
@@ -2225,13 +2330,13 @@
       <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="55">
+      <c r="C39" s="54">
         <v>42802</v>
       </c>
       <c r="D39" s="40"/>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
-      <c r="G39" s="64"/>
+      <c r="G39" s="62"/>
       <c r="H39" s="27"/>
       <c r="I39" s="18"/>
     </row>
@@ -2239,13 +2344,13 @@
       <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="55">
+      <c r="C40" s="54">
         <v>42803</v>
       </c>
       <c r="D40" s="40"/>
       <c r="E40" s="40"/>
       <c r="F40" s="40"/>
-      <c r="G40" s="64"/>
+      <c r="G40" s="62"/>
       <c r="H40" s="27"/>
       <c r="I40" s="18"/>
     </row>
@@ -2253,17 +2358,17 @@
       <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="55">
+      <c r="C41" s="54">
         <v>42804</v>
       </c>
       <c r="D41" s="40"/>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
-      <c r="G41" s="64"/>
+      <c r="G41" s="62"/>
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
@@ -2277,107 +2382,138 @@
         <f>SUM(F37:F41)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="65"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="35" t="s">
+    <row r="43" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="54">
+        <v>42814</v>
+      </c>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="54">
+        <v>42815</v>
+      </c>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="54">
+        <v>42816</v>
+      </c>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="54">
+        <v>42817</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="2:9" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="54">
+        <v>42818</v>
+      </c>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="2:9" s="14" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42">
+        <f>SUM(D43:D47)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42">
+        <f>SUM(F43:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="51"/>
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="2:8" s="14" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="9"/>
+      <c r="C49" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D49" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
         <v>30</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36">
+      <c r="E49" s="36"/>
+      <c r="F49" s="36">
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="9"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="67" t="s">
+      <c r="G49" s="52"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="9"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.25">
+      <c r="B52" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="68"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="59" t="s">
+      <c r="C52" s="68"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-    </row>
-    <row r="47" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-    </row>
-    <row r="48" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-    </row>
-    <row r="49" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="8"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="8"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="8"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="G52" s="21"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
@@ -2389,7 +2525,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2400,22 +2536,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="23"/>
-    <col min="3" max="3" width="11.7109375" style="13" customWidth="1"/>
-    <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="23"/>
+    <col min="3" max="3" width="11.6640625" style="13" customWidth="1"/>
+    <col min="4" max="6" width="11.88671875" style="13" customWidth="1"/>
     <col min="7" max="7" width="33" style="53" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="53" customWidth="1"/>
-    <col min="9" max="16384" width="13.42578125" style="13"/>
+    <col min="8" max="8" width="10.5546875" style="53" customWidth="1"/>
+    <col min="9" max="16384" width="13.44140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
@@ -2426,7 +2562,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2435,7 +2571,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
         <v>17</v>
       </c>
@@ -2451,7 +2587,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="1"/>
       <c r="F6" s="32"/>
@@ -2472,7 +2608,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2523,7 +2659,7 @@
       <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="54">
         <v>42772</v>
       </c>
       <c r="D13" s="39">
@@ -2531,7 +2667,7 @@
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="56" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="27"/>
@@ -2542,7 +2678,7 @@
       <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="54">
         <v>42773</v>
       </c>
       <c r="D14" s="40"/>
@@ -2558,7 +2694,7 @@
       <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="55">
+      <c r="C15" s="54">
         <v>42774</v>
       </c>
       <c r="D15" s="40">
@@ -2566,7 +2702,7 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="57" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="27"/>
@@ -2576,7 +2712,7 @@
       <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="54">
         <v>42775</v>
       </c>
       <c r="D16" s="40">
@@ -2584,7 +2720,7 @@
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="58" t="s">
+      <c r="G16" s="57" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="27"/>
@@ -2594,7 +2730,7 @@
       <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="55">
+      <c r="C17" s="54">
         <v>42776</v>
       </c>
       <c r="D17" s="40">
@@ -2602,7 +2738,7 @@
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="27"/>
@@ -2633,7 +2769,7 @@
       <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="55">
+      <c r="C19" s="54">
         <v>42779</v>
       </c>
       <c r="D19" s="39"/>
@@ -2647,7 +2783,7 @@
       <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="54">
         <v>42780</v>
       </c>
       <c r="D20" s="40"/>
@@ -2661,7 +2797,7 @@
       <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="55">
+      <c r="C21" s="54">
         <v>42781</v>
       </c>
       <c r="D21" s="40"/>
@@ -2675,7 +2811,7 @@
       <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="54">
         <v>42782</v>
       </c>
       <c r="D22" s="40"/>
@@ -2689,7 +2825,7 @@
       <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="55">
+      <c r="C23" s="54">
         <v>42783</v>
       </c>
       <c r="D23" s="40"/>
@@ -2721,7 +2857,7 @@
       <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="55">
+      <c r="C25" s="54">
         <v>42793</v>
       </c>
       <c r="D25" s="39">
@@ -2739,7 +2875,7 @@
       <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="54">
         <v>42794</v>
       </c>
       <c r="D26" s="40"/>
@@ -2753,7 +2889,7 @@
       <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="54">
         <v>42795</v>
       </c>
       <c r="D27" s="40">
@@ -2771,7 +2907,7 @@
       <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="54">
         <v>42796</v>
       </c>
       <c r="D28" s="40">
@@ -2789,7 +2925,7 @@
       <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="54">
         <v>42797</v>
       </c>
       <c r="D29" s="40"/>
@@ -2803,7 +2939,7 @@
       <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="55"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
         <v>11</v>
@@ -2821,7 +2957,7 @@
       <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="55">
+      <c r="C31" s="54">
         <v>42800</v>
       </c>
       <c r="D31" s="39">
@@ -2839,7 +2975,7 @@
       <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="54">
         <v>42801</v>
       </c>
       <c r="D32" s="40">
@@ -2857,7 +2993,7 @@
       <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="55">
+      <c r="C33" s="54">
         <v>42802</v>
       </c>
       <c r="D33" s="40"/>
@@ -2871,7 +3007,7 @@
       <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <v>42803</v>
       </c>
       <c r="D34" s="40"/>
@@ -2885,7 +3021,7 @@
       <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="55">
+      <c r="C35" s="54">
         <v>42804</v>
       </c>
       <c r="D35" s="40"/>
@@ -2917,7 +3053,7 @@
       <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="55"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
@@ -2929,7 +3065,7 @@
       <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="55"/>
+      <c r="C38" s="54"/>
       <c r="D38" s="40"/>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
@@ -2941,7 +3077,7 @@
       <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="55"/>
+      <c r="C39" s="54"/>
       <c r="D39" s="40"/>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
@@ -2953,7 +3089,7 @@
       <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="55"/>
+      <c r="C40" s="54"/>
       <c r="D40" s="40"/>
       <c r="E40" s="40"/>
       <c r="F40" s="40"/>
@@ -2965,7 +3101,7 @@
       <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="55"/>
+      <c r="C41" s="54"/>
       <c r="D41" s="40"/>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
@@ -2973,7 +3109,7 @@
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
@@ -2991,103 +3127,134 @@
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="35" t="s">
+    <row r="43" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="54">
+        <v>42814</v>
+      </c>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="54">
+        <v>42815</v>
+      </c>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="54">
+        <v>42816</v>
+      </c>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="54">
+        <v>42817</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="2:9" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="54">
+        <v>42818</v>
+      </c>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="2:9" s="14" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42">
+        <f>SUM(D43:D47)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42">
+        <f>SUM(F43:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="51"/>
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="2:8" s="14" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="9"/>
+      <c r="C49" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D49" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
         <v>30</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36">
+      <c r="E49" s="36"/>
+      <c r="F49" s="36">
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="9"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="67" t="s">
+      <c r="G49" s="52"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="9"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="68"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="59" t="s">
+      <c r="C52" s="68"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-    </row>
-    <row r="47" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-    </row>
-    <row r="48" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-    </row>
-    <row r="49" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="8"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="8"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="8"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="G52" s="21"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
@@ -3099,7 +3266,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3110,21 +3277,21 @@
   <dimension ref="B2:I53"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B42" sqref="B42:G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="23"/>
-    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="23"/>
+    <col min="3" max="3" width="9.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.88671875" style="13" customWidth="1"/>
     <col min="7" max="7" width="33" style="53" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="53" customWidth="1"/>
-    <col min="9" max="16384" width="13.42578125" style="13"/>
+    <col min="8" max="8" width="10.5546875" style="53" customWidth="1"/>
+    <col min="9" max="16384" width="13.44140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
@@ -3135,7 +3302,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3144,7 +3311,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="s">
         <v>18</v>
       </c>
@@ -3160,7 +3327,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="12" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="1"/>
       <c r="F6" s="32"/>
@@ -3181,7 +3348,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3232,7 +3399,7 @@
       <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="60">
+      <c r="C13" s="58">
         <v>42772</v>
       </c>
       <c r="D13" s="39">
@@ -3250,7 +3417,7 @@
       <c r="B14" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="60">
+      <c r="C14" s="58">
         <v>42773</v>
       </c>
       <c r="D14" s="40"/>
@@ -3264,7 +3431,7 @@
       <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="60">
+      <c r="C15" s="58">
         <v>42774</v>
       </c>
       <c r="D15" s="40"/>
@@ -3278,7 +3445,7 @@
       <c r="B16" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="60">
+      <c r="C16" s="58">
         <v>42775</v>
       </c>
       <c r="D16" s="40"/>
@@ -3292,7 +3459,7 @@
       <c r="B17" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="60">
+      <c r="C17" s="58">
         <v>42776</v>
       </c>
       <c r="D17" s="40"/>
@@ -3327,7 +3494,7 @@
       <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="60">
+      <c r="C19" s="58">
         <v>42779</v>
       </c>
       <c r="D19" s="39"/>
@@ -3341,7 +3508,7 @@
       <c r="B20" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="60">
+      <c r="C20" s="58">
         <v>42780</v>
       </c>
       <c r="D20" s="40"/>
@@ -3355,7 +3522,7 @@
       <c r="B21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="60">
+      <c r="C21" s="58">
         <v>42781</v>
       </c>
       <c r="D21" s="40"/>
@@ -3369,7 +3536,7 @@
       <c r="B22" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="60">
+      <c r="C22" s="58">
         <v>42782</v>
       </c>
       <c r="D22" s="40"/>
@@ -3383,7 +3550,7 @@
       <c r="B23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="60">
+      <c r="C23" s="58">
         <v>42783</v>
       </c>
       <c r="D23" s="40"/>
@@ -3415,7 +3582,7 @@
       <c r="B25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="55">
+      <c r="C25" s="54">
         <v>42793</v>
       </c>
       <c r="D25" s="39"/>
@@ -3429,7 +3596,7 @@
       <c r="B26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="54">
         <v>42794</v>
       </c>
       <c r="D26" s="40"/>
@@ -3443,7 +3610,7 @@
       <c r="B27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="54">
         <v>42795</v>
       </c>
       <c r="D27" s="40"/>
@@ -3457,7 +3624,7 @@
       <c r="B28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="54">
         <v>42796</v>
       </c>
       <c r="D28" s="40"/>
@@ -3471,7 +3638,7 @@
       <c r="B29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="55">
+      <c r="C29" s="54">
         <v>42797</v>
       </c>
       <c r="D29" s="40"/>
@@ -3485,7 +3652,7 @@
       <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="55"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="42">
         <f>SUM(D25:D29)</f>
         <v>0</v>
@@ -3503,7 +3670,7 @@
       <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="55">
+      <c r="C31" s="54">
         <v>42800</v>
       </c>
       <c r="D31" s="39"/>
@@ -3517,7 +3684,7 @@
       <c r="B32" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="54">
         <v>42801</v>
       </c>
       <c r="D32" s="40"/>
@@ -3531,7 +3698,7 @@
       <c r="B33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="55">
+      <c r="C33" s="54">
         <v>42802</v>
       </c>
       <c r="D33" s="40"/>
@@ -3545,7 +3712,7 @@
       <c r="B34" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <v>42803</v>
       </c>
       <c r="D34" s="40"/>
@@ -3559,7 +3726,7 @@
       <c r="B35" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="55">
+      <c r="C35" s="54">
         <v>42804</v>
       </c>
       <c r="D35" s="40"/>
@@ -3591,7 +3758,7 @@
       <c r="B37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="60"/>
+      <c r="C37" s="58"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
@@ -3603,7 +3770,7 @@
       <c r="B38" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="60"/>
+      <c r="C38" s="58"/>
       <c r="D38" s="40"/>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
@@ -3615,7 +3782,7 @@
       <c r="B39" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="60"/>
+      <c r="C39" s="58"/>
       <c r="D39" s="40"/>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
@@ -3627,7 +3794,7 @@
       <c r="B40" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="60"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="40"/>
       <c r="E40" s="40"/>
       <c r="F40" s="40"/>
@@ -3639,7 +3806,7 @@
       <c r="B41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="60"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="40"/>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
@@ -3647,7 +3814,7 @@
       <c r="H41" s="27"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="20" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="45" t="s">
         <v>33</v>
       </c>
@@ -3665,103 +3832,134 @@
       <c r="H42" s="28"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="35" t="s">
+    <row r="43" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="54">
+        <v>42814</v>
+      </c>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="54">
+        <v>42815</v>
+      </c>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="54">
+        <v>42816</v>
+      </c>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="54">
+        <v>42817</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="54">
+        <v>42818</v>
+      </c>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="2:9" s="14" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="41"/>
+      <c r="D48" s="42">
+        <f>SUM(D43:D47)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42">
+        <f>SUM(F43:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="51"/>
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="2:8" s="14" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="9"/>
+      <c r="C49" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D49" s="36">
         <f>SUM(D18+D24+D30+D36+D42)</f>
         <v>5</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36">
+      <c r="E49" s="36"/>
+      <c r="F49" s="36">
         <f>SUM(F18+F24+F30+F36+F42)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="9"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="67" t="s">
+      <c r="G49" s="52"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="9"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.25">
+      <c r="B52" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="68"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="59" t="s">
+      <c r="C52" s="68"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-    </row>
-    <row r="47" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-    </row>
-    <row r="48" spans="2:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-    </row>
-    <row r="49" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="8"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="8"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="8"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="G52" s="21"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
@@ -3773,7 +3971,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>